<commit_message>
change report templates 16022022
</commit_message>
<xml_diff>
--- a/web/excel/qarzdor.xlsx
+++ b/web/excel/qarzdor.xlsx
@@ -5,30 +5,133 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Avaz\Соглом\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Web\OpenServer\domains\soglomdi\web\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2C09624-16D5-462F-A4C9-62A63CD0D374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A16FAA8-4AEB-4817-9FC6-C8E8BAE9D34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Пользователь</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Пользователь:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Янги кушилди</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Пользователь:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Янги кушилди</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Пользователь:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Янги кушилди</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Пользователь:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Бунда автомат карзга утиши керак. Регистратор карзга олиб борса-бормаса</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Бемор карздорлиги</t>
   </si>
   <si>
-    <t>2022-01-01</t>
-  </si>
-  <si>
-    <t>2022-02-02</t>
+    <t>2022-02-11</t>
   </si>
   <si>
     <t>all</t>
@@ -74,6 +177,15 @@
   </si>
   <si>
     <t>Реферал тел раками</t>
+  </si>
+  <si>
+    <t>Филиал номи</t>
+  </si>
+  <si>
+    <t>Статус</t>
+  </si>
+  <si>
+    <t>Анализ суммаси</t>
   </si>
 </sst>
 </file>
@@ -81,9 +193,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -93,16 +205,25 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF003F2F"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -117,14 +238,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA9CD90"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFD6E5CB"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD6E5CB"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor rgb="FFA9CD90"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -160,18 +281,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -477,104 +598,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="44" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="26.5546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="3"/>
+    <col min="2" max="3" width="41.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="44" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="18.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="15" style="5" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" style="5" customWidth="1"/>
+    <col min="15" max="15" width="26.5546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="33.5546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="21.44140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7"/>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>17</v>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>